<commit_message>
add init script for postgres add postgres document & data structure
</commit_message>
<xml_diff>
--- a/document/dataStructure.xlsx
+++ b/document/dataStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shinya\development\github\no1-company-share\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0929930-F688-4FBD-857C-DCD4B8B66434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A23ECE-1020-4D07-811E-516C1F671B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>物理名</t>
     <rPh sb="0" eb="3">
@@ -169,13 +169,6 @@
     <t>http://a3.example.com</t>
   </si>
   <si>
-    <t>投稿№</t>
-    <rPh sb="0" eb="3">
-      <t>トウコウナンバー</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>P001</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -209,16 +202,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>投稿詳細№</t>
-    <rPh sb="0" eb="2">
-      <t>トウコウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>一位区分</t>
     <rPh sb="0" eb="2">
       <t>イチイ</t>
@@ -243,6 +226,112 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>xxx</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>△△△</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お気に入り</t>
+    <rPh sb="1" eb="2">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bookmark</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お気に入りユーザID</t>
+    <rPh sb="1" eb="2">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YAMADA</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿ID</t>
+  </si>
+  <si>
+    <t>投稿ID</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿詳細ID</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>区分値マスタ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>区分ID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>区分値名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NO1_DIVISION</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>WORLD_NO1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カラム名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>区分名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>JAPAN_NO1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FUKUI_NO1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>世界一</t>
+    <rPh sb="0" eb="3">
+      <t>セカイイチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>日本一</t>
     <rPh sb="0" eb="3">
       <t>ニホンイチ</t>
@@ -250,53 +339,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>世界一</t>
-    <rPh sb="0" eb="3">
-      <t>セカイイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>福井一</t>
     <rPh sb="0" eb="3">
       <t>フクイイチ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xxx</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>△△△</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お気に入り</t>
-    <rPh sb="1" eb="2">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>イ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Bookmark</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お気に入りユーザID</t>
-    <rPh sb="1" eb="2">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>イ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>YAMADA</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -707,10 +753,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.7">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -722,38 +768,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A1A741-3647-43DB-9FA0-3A15221292F8}">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
   <cols>
     <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.0625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" customWidth="1"/>
+    <col min="4" max="4" width="13.6875" customWidth="1"/>
+    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.4375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.0625" customWidth="1"/>
+    <col min="11" max="11" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.8125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.7">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.7">
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.7">
       <c r="C3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.7">
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.7">
       <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.7">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.7">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -767,7 +920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.7">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.7">
       <c r="C7" t="s">
         <v>16</v>
       </c>
@@ -777,8 +930,23 @@
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.7">
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.7">
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -788,8 +956,20 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.7">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.7">
       <c r="C9" t="s">
         <v>24</v>
       </c>
@@ -799,229 +979,146 @@
       <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.7">
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.7">
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.7">
-      <c r="C12" t="s">
+      <c r="J15" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.7">
+      <c r="I16" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.7">
-      <c r="C13" t="s">
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.7">
+      <c r="I17" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.7">
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.7">
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.7">
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1033,5 +1130,6 @@
     <hyperlink ref="E9" r:id="rId3" display="http://a2.example.com" xr:uid="{75F0A050-3608-4D3C-8A8F-27B1BE1BF401}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add sample data for bookmark table
</commit_message>
<xml_diff>
--- a/document/dataStructure.xlsx
+++ b/document/dataStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shinya\development\github\no1-company-share\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A23ECE-1020-4D07-811E-516C1F671B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82C72CC-8F48-40E6-A7E5-958CD4517466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>物理名</t>
     <rPh sb="0" eb="3">
@@ -768,7 +768,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A1A741-3647-43DB-9FA0-3A15221292F8}">
-  <dimension ref="B1:O17"/>
+  <dimension ref="B1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.7">
       <c r="I16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J16" t="s">
         <v>41</v>
@@ -1116,9 +1116,17 @@
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.7">
       <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.7">
+      <c r="I18" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#11 add spec for api data
</commit_message>
<xml_diff>
--- a/document/dataStructure.xlsx
+++ b/document/dataStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shinya\development\github\no1-company-share\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82C72CC-8F48-40E6-A7E5-958CD4517466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A33279-CD9F-4DE4-8E3C-37A9D057BBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10876" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>物理名</t>
     <rPh sb="0" eb="3">
@@ -305,23 +305,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>WORLD_NO1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>カラム名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>区分名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>JAPAN_NO1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FUKUI_NO1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1014,12 +998,9 @@
         <v>47</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I11">
@@ -1043,10 +1024,7 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1069,10 +1047,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.7">
@@ -1083,10 +1058,7 @@
         <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>38</v>

</xml_diff>